<commit_message>
rely on original entice3 data 'mistakes'
</commit_message>
<xml_diff>
--- a/data/Dummy infographics data.xlsx
+++ b/data/Dummy infographics data.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -85,7 +82,7 @@
     <t xml:space="preserve">promis_anxiety_t</t>
   </si>
   <si>
-    <t xml:space="preserve">promis_depression_t</t>
+    <t xml:space="preserve">proms_depression_t</t>
   </si>
   <si>
     <t xml:space="preserve">sf_1</t>
@@ -166,6 +163,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -243,7 +241,7 @@
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -252,100 +250,97 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="T1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="U1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="X1" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="Y1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Z1" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="AA1" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="AA1" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>19</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>14.8</v>
@@ -419,16 +414,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>28</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>21</v>
@@ -502,16 +497,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>51</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>29</v>
@@ -585,16 +580,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>62</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>38.5</v>
@@ -668,16 +663,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>82</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>24.9</v>

</xml_diff>

<commit_message>
values need to be rounded
</commit_message>
<xml_diff>
--- a/data/Dummy infographics data.xlsx
+++ b/data/Dummy infographics data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sample6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample7</t>
   </si>
 </sst>
 </file>
@@ -249,13 +252,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA8"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.61133603238866"/>
   </cols>
@@ -838,11 +841,94 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>53</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="K8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="R8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U8" s="4" t="n">
+        <v>51.2</v>
+      </c>
+      <c r="V8" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="W8" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="X8" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="4" t="n">
+        <v>106</v>
+      </c>
+      <c r="Z8" s="4" t="n">
+        <v>68</v>
+      </c>
+      <c r="AA8" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>